<commit_message>
fixed acq_join function to work with a square range
</commit_message>
<xml_diff>
--- a/ACQ.Excel/Examples/ACQ.Stats.xlsx
+++ b/ACQ.Excel/Examples/ACQ.Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803685A-BE9A-465A-A3BD-3753544475A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C286022C-4C69-459A-B943-C9AF50140F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="1755" windowWidth="24450" windowHeight="12690" tabRatio="900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>date</t>
   </si>
@@ -200,6 +200,21 @@
   </si>
   <si>
     <t>acq_sumofsquares</t>
+  </si>
+  <si>
+    <t>acq_count</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>text3</t>
+  </si>
+  <si>
+    <t>Is64 Bit Process</t>
+  </si>
+  <si>
+    <t>Number of Logical Cores</t>
   </si>
 </sst>
 </file>
@@ -787,12 +802,12 @@
   <dimension ref="B2:N56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" customWidth="1"/>
@@ -839,7 +854,7 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.5.8035.39108</v>
+        <v>1.5.8035.39699</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -910,6 +925,13 @@
       </c>
     </row>
     <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="6" t="b">
+        <f>_xll.acq_is64bit()</f>
+        <v>1</v>
+      </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
@@ -922,11 +944,14 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3"/>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="6">
+        <f>_xll.acq_cpu_cores()</f>
+        <v>32</v>
+      </c>
       <c r="G9" t="s">
         <v>21</v>
       </c>
@@ -940,12 +965,6 @@
       </c>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="G10" t="s">
         <v>24</v>
       </c>
@@ -958,15 +977,27 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" t="s">
+    <row r="11" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" ht="15.75" thickBot="1">
       <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
@@ -2190,10 +2221,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30B9D5F-797C-49CC-9435-B3BF433B0ECB}">
-  <dimension ref="B1:L18"/>
+  <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2218,11 +2249,11 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">_xll.acq_min(H2:L18)</f>
-        <v>-0.997</v>
+        <v>-0.94599999999999995</v>
       </c>
       <c r="D2" s="6">
         <f t="array" aca="1" ref="D2" ca="1">MIN(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>-0.997</v>
+        <v>-0.94599999999999995</v>
       </c>
       <c r="E2">
         <f ca="1">C2-D2</f>
@@ -2230,23 +2261,23 @@
       </c>
       <c r="H2" s="5">
         <f ca="1">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>0.311</v>
+        <v>0.33</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:L18" ca="1" si="0">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>0.81699999999999995</v>
+        <v>0.439</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65500000000000003</v>
+        <v>-0.51400000000000001</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.25600000000000001</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.65800000000000003</v>
+        <v>-0.14499999999999999</v>
       </c>
     </row>
     <row r="3" spans="2:12">
@@ -2255,35 +2286,35 @@
       </c>
       <c r="C3" s="6">
         <f ca="1">_xll.acq_absmin(H2:L18)</f>
-        <v>4.2999999999999997E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D3" s="6">
         <f t="array" aca="1" ref="D3" ca="1">MIN(ABS(IF(ISNUMBER(H2:L18), H2:L18)))</f>
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E10" ca="1" si="1">C3-D3</f>
-        <v>4.2999999999999997E-2</v>
+        <f t="shared" ref="E3:E11" ca="1" si="1">C3-D3</f>
+        <v>0.04</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ref="H3:H18" ca="1" si="2">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>0.85199999999999998</v>
+        <v>-0.90100000000000002</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.46200000000000002</v>
+        <v>-0.85399999999999998</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.63700000000000001</v>
+        <v>-0.85</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76400000000000001</v>
+        <v>-0.81299999999999994</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28499999999999998</v>
+        <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="4" spans="2:12">
@@ -2292,11 +2323,11 @@
       </c>
       <c r="C4" s="6">
         <f ca="1">_xll.acq_max(H2:L18)</f>
-        <v>0.996</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="D4" s="6">
         <f t="array" aca="1" ref="D4" ca="1">MAX(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>0.996</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
@@ -2304,22 +2335,22 @@
       </c>
       <c r="H4" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.89800000000000002</v>
+        <v>-7.1999999999999995E-2</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.217</v>
+        <v>0.05</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85399999999999998</v>
+        <v>-0.61799999999999999</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96199999999999997</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="5" spans="2:12">
@@ -2328,11 +2359,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">_xll.acq_absmax(H2:L18)</f>
-        <v>0.997</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="D5" s="6">
         <f t="array" aca="1" ref="D5" ca="1">MAX(ABS(IF(ISNUMBER(H2:L18), H2:L18)))</f>
-        <v>0.997</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
@@ -2340,22 +2371,22 @@
       </c>
       <c r="H5" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.97299999999999998</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.104</v>
+        <v>0.78600000000000003</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.68500000000000005</v>
+        <v>-0.86799999999999999</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.75700000000000001</v>
+        <v>-0.13900000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:12">
@@ -2364,11 +2395,11 @@
       </c>
       <c r="C6" s="6">
         <f ca="1">_xll.acq_sum(H2:L18)</f>
-        <v>2.5649999999999995</v>
+        <v>-2.488</v>
       </c>
       <c r="D6" s="6">
         <f t="array" aca="1" ref="D6" ca="1">SUM(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>2.5650000000000004</v>
+        <v>-2.4879999999999995</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -2376,23 +2407,22 @@
       </c>
       <c r="H6" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88</v>
-      </c>
-      <c r="I6" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>-0.41199999999999998</v>
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2999999999999997E-2</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.435</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99399999999999999</v>
+        <v>-0.27100000000000002</v>
       </c>
     </row>
     <row r="7" spans="2:12">
@@ -2400,36 +2430,35 @@
         <v>25</v>
       </c>
       <c r="C7" s="6">
-        <f ca="1">_xll.acq_count_unique(H2:L18, TRUE)</f>
-        <v>77</v>
+        <f ca="1">_xll.acq_count_unique(H2:L18)</f>
+        <v>79</v>
       </c>
       <c r="D7" s="6">
         <f t="array" aca="1" ref="D7" ca="1">COUNT(H2:L18)</f>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>-0.52700000000000002</v>
+        <v>-0.311</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8000000000000005E-2</v>
+        <v>-0.85799999999999998</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.45500000000000002</v>
+        <v>-0.62</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.221</v>
+        <v>0.54200000000000004</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -2438,11 +2467,11 @@
       </c>
       <c r="C8" s="6">
         <f ca="1">_xll.acq_mean(H2:L18)</f>
-        <v>3.288461538461538E-2</v>
+        <v>-3.2736842105263154E-2</v>
       </c>
       <c r="D8" s="6">
         <f t="array" aca="1" ref="D8" ca="1">AVERAGE(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>3.2884615384615387E-2</v>
+        <v>-3.2736842105263154E-2</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
@@ -2450,23 +2479,23 @@
       </c>
       <c r="H8" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.58299999999999996</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.93700000000000006</v>
+        <v>-0.69499999999999995</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48099999999999998</v>
+        <v>-0.94599999999999995</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27300000000000002</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.41399999999999998</v>
+        <v>-0.85899999999999999</v>
       </c>
     </row>
     <row r="9" spans="2:12">
@@ -2475,11 +2504,11 @@
       </c>
       <c r="C9" s="6">
         <f ca="1">_xll.acq_stdev(H2:L18)</f>
-        <v>0.6517717706827606</v>
+        <v>0.58206458675811457</v>
       </c>
       <c r="D9" s="6">
         <f t="array" aca="1" ref="D9" ca="1">_xlfn.STDEV.S(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>0.6517717706827606</v>
+        <v>0.58206458675811457</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
@@ -2487,22 +2516,22 @@
       </c>
       <c r="H9" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.129</v>
+        <v>0.04</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81699999999999995</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47199999999999998</v>
+        <v>0.626</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64200000000000002</v>
+        <v>-0.50800000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -2511,11 +2540,11 @@
       </c>
       <c r="C10" s="6">
         <f ca="1">_xll.acq_sumofsquares(H2:L18)</f>
-        <v>32.794444999999996</v>
+        <v>25.491387999999997</v>
       </c>
       <c r="D10" s="6">
         <f t="array" aca="1" ref="D10" ca="1">SUM(IF(ISNUMBER(H2:L18), H2:L18^2))</f>
-        <v>32.794444999999996</v>
+        <v>25.491388000000001</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
@@ -2523,11 +2552,11 @@
       </c>
       <c r="H10" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.57899999999999996</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.996</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="J10" s="5" t="e">
         <f>1/0</f>
@@ -2535,184 +2564,227 @@
       </c>
       <c r="K10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.877</v>
+        <v>-8.5000000000000006E-2</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.77200000000000002</v>
+        <v>0.17199999999999999</v>
       </c>
     </row>
     <row r="11" spans="2:12">
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="6">
+        <f ca="1">_xll.acq_count(H2:L18)</f>
+        <v>76</v>
+      </c>
+      <c r="D11" s="6">
+        <f ca="1">COUNT(H2:L18)</f>
+        <v>76</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H11" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.97899999999999998</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.70599999999999996</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>49</v>
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="J11" s="5" t="e">
+        <f>SQRT(-1)</f>
+        <v>#NUM!</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11799999999999999</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.58499999999999996</v>
+        <v>0.97099999999999997</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="H12" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.74199999999999999</v>
+        <v>-0.81</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.68600000000000005</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.65900000000000003</v>
+        <v>-0.192</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>0.29399999999999998</v>
       </c>
     </row>
     <row r="13" spans="2:12">
       <c r="H13" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.81399999999999995</v>
+        <v>-0.106</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.73499999999999999</v>
+        <v>-0.90900000000000003</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.27300000000000002</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.56499999999999995</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.20599999999999999</v>
+        <v>0.88200000000000001</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="H14" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22600000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.90800000000000003</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34899999999999998</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.73499999999999999</v>
+        <v>-0.1</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.72199999999999998</v>
+        <v>-5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="H15" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.40200000000000002</v>
+        <v>-0.64300000000000002</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.629</v>
+        <v>0.498</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79500000000000004</v>
+        <v>-0.128</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.997</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22600000000000001</v>
+        <v>-0.64100000000000001</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="H16" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.57199999999999995</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85699999999999998</v>
+        <v>-0.67</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.89300000000000002</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23499999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="8:12">
+        <v>-0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="H17" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16</v>
+        <v>-0.76100000000000001</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91400000000000003</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86099999999999999</v>
+        <v>-0.85899999999999999</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.871</v>
+        <v>-0.26600000000000001</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64800000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="8:12">
+        <v>-0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="H18" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.52400000000000002</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.66500000000000004</v>
+        <v>-9.4E-2</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62</v>
+        <v>-0.65700000000000003</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58699999999999997</v>
+        <v>-0.71299999999999997</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82299999999999995</v>
+        <v>-0.63600000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="str">
+        <f ca="1">_xll.acq_join(H2:L18, "|")</f>
+        <v>0.33|-0.901|-0.072|0.178|0.204|-0.311|0.815|0.04|0.416|0.148|-0.81|-0.106|0.22|-0.643|0.863|-0.761|0.519|0.439|-0.854|0.05|text|text|text3|-0.695|0.857|0.712|0.895|0.593|-0.909|0.609|0.498|text|0.077|-0.094|-0.514|-0.85|-0.618|0.786|0.451|-0.858|-0.946|text|||text|0.858|0.428|-0.128|-0.67|-0.859|-0.657|0.574|-0.813|text2|-0.868|-0.044|-0.62|0.582|0.626|-0.085|0.163|-0.192|0.174|-0.1|0.965|0.466|-0.266|-0.713|-0.145|0.101|0.098|-0.139|-0.271|0.542|-0.859|-0.508|0.172|0.971|0.294|0.882|-0.053|-0.641|-0.525|-0.35|-0.636</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="str">
+        <f ca="1">_xll.acq_join(J2:J18, "|")</f>
+        <v>-0.514|-0.85|-0.618|0.786|0.451|-0.858|-0.946|text|||text|0.858|0.428|-0.128|-0.67|-0.859|-0.657</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="str">
+        <f ca="1">_xll.acq_join(H7:L7, "|")</f>
+        <v>-0.311|text3|-0.858|-0.62|0.542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>